<commit_message>
Added DataModel & Updated .xls file
</commit_message>
<xml_diff>
--- a/data/Database_Info.xlsx
+++ b/data/Database_Info.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PixelSoftware\Macos_Updated\ADSNL_MACOS_Updated\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PixelSoftware\Macos_Updated\ADSNL_MACOS_Updated\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D5AA7D-34B3-4D5F-8B0F-A9220E3F8293}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FB4E44-50BF-4E2F-89C3-08E49508A8EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" xr2:uid="{E92C6248-CB53-41C7-806D-C6D89F151F87}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="107">
   <si>
     <t>Books</t>
   </si>
@@ -93,9 +94,6 @@
     <t>Kitchen_Product_ID</t>
   </si>
   <si>
-    <t>Makup</t>
-  </si>
-  <si>
     <t>Makeup_Category_ID</t>
   </si>
   <si>
@@ -234,18 +232,12 @@
     <t>Brand/Publisher/Manufacturer</t>
   </si>
   <si>
-    <t>Genre</t>
-  </si>
-  <si>
     <t>Author</t>
   </si>
   <si>
     <t>Author_Lookup</t>
   </si>
   <si>
-    <t>Category/Type</t>
-  </si>
-  <si>
     <t>Prod_SKU</t>
   </si>
   <si>
@@ -265,6 +257,102 @@
   </si>
   <si>
     <t>Size_Lookup</t>
+  </si>
+  <si>
+    <t>Makeup</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Type_Lookup</t>
+  </si>
+  <si>
+    <t>Category/Genre</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Customer_ID</t>
+  </si>
+  <si>
+    <t>Customer_FName</t>
+  </si>
+  <si>
+    <t>Customer_LName</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Birth_Date</t>
+  </si>
+  <si>
+    <t>Zip_Code</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Street_Number</t>
+  </si>
+  <si>
+    <t>Street_Name</t>
+  </si>
+  <si>
+    <t>Marital_Status_Type</t>
+  </si>
+  <si>
+    <t>Street_Type_Lookup</t>
+  </si>
+  <si>
+    <t>Degree_Lookup</t>
+  </si>
+  <si>
+    <t>Income_Lookup</t>
+  </si>
+  <si>
+    <t>Credit_Card_Type</t>
+  </si>
+  <si>
+    <t>ChartData</t>
+  </si>
+  <si>
+    <t>Data_ID</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Order_Count</t>
+  </si>
+  <si>
+    <t>Order_Master</t>
+  </si>
+  <si>
+    <t>Order_ID</t>
+  </si>
+  <si>
+    <t>Order_DateTime</t>
+  </si>
+  <si>
+    <t>Order_Details</t>
+  </si>
+  <si>
+    <t>Customer_ID (PK)</t>
+  </si>
+  <si>
+    <t>Order_Detail_ID</t>
+  </si>
+  <si>
+    <t>Product_ID</t>
+  </si>
+  <si>
+    <t>Product_Media_ID</t>
   </si>
 </sst>
 </file>
@@ -303,7 +391,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,6 +416,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -341,12 +435,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -355,6 +446,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204D7EE7-66FC-40EC-ACD6-D52879A47543}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -683,32 +778,48 @@
     <col min="5" max="5" width="20.90625" customWidth="1"/>
     <col min="6" max="6" width="22.90625" customWidth="1"/>
     <col min="8" max="8" width="31.6328125" customWidth="1"/>
+    <col min="9" max="9" width="27.90625" customWidth="1"/>
+    <col min="10" max="10" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.6328125" customWidth="1"/>
+    <col min="12" max="12" width="21.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -719,19 +830,31 @@
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+      <c r="I2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -742,19 +865,31 @@
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+      <c r="I3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -765,19 +900,31 @@
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+      <c r="I4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" t="s">
+        <v>98</v>
+      </c>
+      <c r="K4" t="s">
+        <v>103</v>
+      </c>
+      <c r="L4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -788,19 +935,25 @@
         <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="I5" t="s">
+        <v>83</v>
+      </c>
+      <c r="L5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -811,16 +964,22 @@
         <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" t="s">
+        <v>84</v>
+      </c>
+      <c r="L6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -828,16 +987,19 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="I7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>14</v>
       </c>
@@ -848,164 +1010,205 @@
         <v>14</v>
       </c>
       <c r="H8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H10" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H10" t="s">
+      <c r="I10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H11" t="s">
+      <c r="I11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H12" t="s">
+        <v>68</v>
+      </c>
+      <c r="I12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="I18" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="K18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>38</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>50</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H19" t="s">
+        <v>78</v>
+      </c>
+      <c r="I19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" t="s">
-        <v>51</v>
-      </c>
-      <c r="H19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
+      <c r="I20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H21" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
+      <c r="I21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="H22" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="6" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B23" t="s">
         <v>48</v>
-      </c>
-      <c r="H22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
       </c>
       <c r="H23" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H26" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H25" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H27" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H26" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H28" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H27" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H28" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H29" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H29" t="s">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H30" s="5" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H30" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H31" s="6" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A16:L16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F04270-17FE-42CD-AB5B-4B51E98E6B8F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Customer & Order tables in Datamodel & .xls
</commit_message>
<xml_diff>
--- a/data/Database_Info.xlsx
+++ b/data/Database_Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PixelSoftware\Macos_Updated\ADSNL_MACOS_Updated\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FB4E44-50BF-4E2F-89C3-08E49508A8EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256AEA1F-BE55-4CAC-9712-4C345F82D671}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" xr2:uid="{E92C6248-CB53-41C7-806D-C6D89F151F87}"/>
   </bookViews>
@@ -446,10 +446,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204D7EE7-66FC-40EC-ACD6-D52879A47543}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1049,20 +1049,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
@@ -1077,7 +1077,7 @@
       <c r="H18" t="s">
         <v>64</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="I18" s="6" t="s">
         <v>91</v>
       </c>
       <c r="K18" t="s">

</xml_diff>

<commit_message>
Updated Data Model & xls file
</commit_message>
<xml_diff>
--- a/data/Database_Info.xlsx
+++ b/data/Database_Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PixelSoftware\Macos_Updated\ADSNL_MACOS_Updated\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19405A5A-BEF2-4690-8D6E-A6816B063A32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88AD56C-1949-44CE-B8BD-20842692A146}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" xr2:uid="{E92C6248-CB53-41C7-806D-C6D89F151F87}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="120">
   <si>
     <t>Books</t>
   </si>
@@ -232,12 +232,6 @@
     <t>Brand/Publisher/Manufacturer</t>
   </si>
   <si>
-    <t>Author</t>
-  </si>
-  <si>
-    <t>Author_Lookup</t>
-  </si>
-  <si>
     <t>Prod_SKU</t>
   </si>
   <si>
@@ -250,15 +244,9 @@
     <t>Color</t>
   </si>
   <si>
-    <t>Color_Lookup</t>
-  </si>
-  <si>
     <t>Size</t>
   </si>
   <si>
-    <t>Size_Lookup</t>
-  </si>
-  <si>
     <t>Makeup</t>
   </si>
   <si>
@@ -392,6 +380,18 @@
   </si>
   <si>
     <t>Makeup_Color_Lookup</t>
+  </si>
+  <si>
+    <t>Author_Director</t>
+  </si>
+  <si>
+    <t>AD_Lookup</t>
+  </si>
+  <si>
+    <t>Feature_Lookup</t>
+  </si>
+  <si>
+    <t>Format</t>
   </si>
 </sst>
 </file>
@@ -803,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204D7EE7-66FC-40EC-ACD6-D52879A47543}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -834,7 +834,7 @@
         <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>26</v>
@@ -846,16 +846,16 @@
         <v>53</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="L1" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -881,16 +881,16 @@
         <v>54</v>
       </c>
       <c r="I2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="J2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K2" t="s">
         <v>96</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>100</v>
-      </c>
-      <c r="L2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
@@ -916,16 +916,16 @@
         <v>55</v>
       </c>
       <c r="I3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K3" t="s">
         <v>97</v>
       </c>
-      <c r="K3" t="s">
-        <v>101</v>
-      </c>
       <c r="L3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -951,16 +951,16 @@
         <v>56</v>
       </c>
       <c r="I4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="K4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="L4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
@@ -986,10 +986,10 @@
         <v>57</v>
       </c>
       <c r="I5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="L5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -1012,7 +1012,7 @@
         <v>59</v>
       </c>
       <c r="I6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L6" t="s">
         <v>14</v>
@@ -1035,7 +1035,7 @@
         <v>60</v>
       </c>
       <c r="I7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -1052,7 +1052,7 @@
         <v>61</v>
       </c>
       <c r="I8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -1060,7 +1060,7 @@
         <v>58</v>
       </c>
       <c r="I9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
@@ -1068,7 +1068,7 @@
         <v>62</v>
       </c>
       <c r="I10" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -1076,15 +1076,15 @@
         <v>63</v>
       </c>
       <c r="I11" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="23.5" x14ac:dyDescent="0.55000000000000004">
@@ -1114,22 +1114,22 @@
         <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E18" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F18" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H18" t="s">
         <v>64</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="K18" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -1143,19 +1143,19 @@
         <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E19" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F19" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I19" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -1169,16 +1169,16 @@
         <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H20" t="s">
         <v>65</v>
       </c>
       <c r="I20" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -1192,16 +1192,16 @@
         <v>52</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E21" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="H21" t="s">
-        <v>66</v>
+        <v>116</v>
       </c>
       <c r="I21" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -1212,13 +1212,13 @@
         <v>47</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E22" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H22" t="s">
-        <v>67</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
@@ -1229,45 +1229,50 @@
         <v>48</v>
       </c>
       <c r="E23" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H26" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H27" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H28" t="s">
-        <v>74</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H29" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H30" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H31" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done With Books Data Migration
</commit_message>
<xml_diff>
--- a/data/Database_Info.xlsx
+++ b/data/Database_Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PixelSoftware\Macos_Updated\ADSNL_MACOS_Updated\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88AD56C-1949-44CE-B8BD-20842692A146}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196DE8BF-9CCB-47A6-93B8-A9DCBCE1F6BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" xr2:uid="{E92C6248-CB53-41C7-806D-C6D89F151F87}"/>
   </bookViews>
@@ -430,7 +430,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -446,12 +446,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -474,9 +468,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -485,7 +478,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -805,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204D7EE7-66FC-40EC-ACD6-D52879A47543}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -823,38 +816,38 @@
     <col min="12" max="12" width="21.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>98</v>
       </c>
     </row>
@@ -938,13 +931,13 @@
       <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="H4" t="s">
@@ -973,13 +966,13 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H5" t="s">
@@ -1002,13 +995,14 @@
       <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>59</v>
       </c>
       <c r="I6" t="s">
@@ -1028,7 +1022,8 @@
       <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
         <v>35</v>
       </c>
       <c r="H7" t="s">
@@ -1045,7 +1040,8 @@
       <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E8" s="4"/>
+      <c r="F8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H8" t="s">
@@ -1088,20 +1084,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
@@ -1125,7 +1121,7 @@
       <c r="H18" t="s">
         <v>64</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="5" t="s">
         <v>87</v>
       </c>
       <c r="K18" t="s">
@@ -1136,7 +1132,7 @@
       <c r="A19" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C19" t="s">
@@ -1159,13 +1155,13 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D20" t="s">
@@ -1182,16 +1178,16 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>114</v>
       </c>
       <c r="E21" t="s">
@@ -1205,13 +1201,13 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>115</v>
       </c>
       <c r="E22" t="s">
@@ -1222,7 +1218,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B23" t="s">
@@ -1261,12 +1257,12 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="H29" s="5" t="s">
+      <c r="H29" s="4" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="H30" s="5" t="s">
+      <c r="H30" s="4" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Python Script Movies tables
</commit_message>
<xml_diff>
--- a/data/Database_Info.xlsx
+++ b/data/Database_Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PixelSoftware\Macos_Updated\ADSNL_MACOS_Updated\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196DE8BF-9CCB-47A6-93B8-A9DCBCE1F6BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B68A2C-705E-421F-ABDA-DEB3170E07A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" xr2:uid="{E92C6248-CB53-41C7-806D-C6D89F151F87}"/>
   </bookViews>
@@ -229,9 +229,6 @@
     <t>Department</t>
   </si>
   <si>
-    <t>Brand/Publisher/Manufacturer</t>
-  </si>
-  <si>
     <t>Prod_SKU</t>
   </si>
   <si>
@@ -392,6 +389,9 @@
   </si>
   <si>
     <t>Format</t>
+  </si>
+  <si>
+    <t>Brand/Publisher/Manufacturer/Movie_Studios</t>
   </si>
 </sst>
 </file>
@@ -798,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204D7EE7-66FC-40EC-ACD6-D52879A47543}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -827,7 +827,7 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>26</v>
@@ -839,16 +839,16 @@
         <v>53</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -874,16 +874,16 @@
         <v>54</v>
       </c>
       <c r="I2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
@@ -909,16 +909,16 @@
         <v>55</v>
       </c>
       <c r="I3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -944,16 +944,16 @@
         <v>56</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
@@ -979,10 +979,10 @@
         <v>57</v>
       </c>
       <c r="I5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -1006,7 +1006,7 @@
         <v>59</v>
       </c>
       <c r="I6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L6" t="s">
         <v>14</v>
@@ -1030,7 +1030,7 @@
         <v>60</v>
       </c>
       <c r="I7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -1048,7 +1048,7 @@
         <v>61</v>
       </c>
       <c r="I8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -1056,7 +1056,7 @@
         <v>58</v>
       </c>
       <c r="I9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
@@ -1064,7 +1064,7 @@
         <v>62</v>
       </c>
       <c r="I10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -1072,15 +1072,15 @@
         <v>63</v>
       </c>
       <c r="I11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="23.5" x14ac:dyDescent="0.55000000000000004">
@@ -1110,22 +1110,22 @@
         <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H18" t="s">
         <v>64</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -1139,19 +1139,19 @@
         <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -1165,16 +1165,16 @@
         <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H20" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="I20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -1188,16 +1188,16 @@
         <v>52</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -1208,13 +1208,13 @@
         <v>47</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
@@ -1225,50 +1225,50 @@
         <v>48</v>
       </c>
       <c r="E23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H29" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H30" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>